<commit_message>
fixed sorting bug inside getApplicantVacancies
</commit_message>
<xml_diff>
--- a/server/db/seeds/Seed_SpreadSheet2.xlsx
+++ b/server/db/seeds/Seed_SpreadSheet2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/behzadazampour/Documents/lighthouse/tempdental/server/db/seeds/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/behzadazampour/Documents/lighthouse/tempdental3/server/db/seeds/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="22100" windowHeight="17460" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22100" windowHeight="17460" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="79">
   <si>
     <t>id</t>
   </si>
@@ -259,6 +259,15 @@
   </si>
   <si>
     <t>2099-01-01</t>
+  </si>
+  <si>
+    <t>anonymous</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>true</t>
   </si>
 </sst>
 </file>
@@ -626,7 +635,7 @@
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f ca="1">CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>mOr7Cpb8c5V</v>
+        <v>oRv4Fus9w5M</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -662,7 +671,7 @@
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>dKw0Ubv7y2U</v>
+        <v>jQd7Whr5a6H</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
@@ -745,7 +754,7 @@
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f ca="1">CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>oOd6Hex7a7A</v>
+        <v>lHt9Sci8h2U</v>
       </c>
       <c r="B2" t="s">
         <v>25</v>
@@ -775,7 +784,7 @@
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>bYj0Xvq9v0N</v>
+        <v>nDx7Mgz0h3E</v>
       </c>
       <c r="B3" t="s">
         <v>26</v>
@@ -809,10 +818,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -823,7 +832,7 @@
     <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -842,11 +851,14 @@
       <c r="F1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f ca="1">CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>uWt2Yzo9m2L</v>
+        <v>iJi9Mle7a6A</v>
       </c>
       <c r="B2" t="s">
         <v>36</v>
@@ -863,11 +875,14 @@
       <c r="F2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A8" ca="1" si="0">CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>yZs5Zkw8t8D</v>
+        <v>sDh6Cit5p4O</v>
       </c>
       <c r="B3" t="s">
         <v>37</v>
@@ -884,11 +899,14 @@
       <c r="F3" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>qIm1Akg7f6R</v>
+        <v>nSm6Icr0i6H</v>
       </c>
       <c r="B4" t="s">
         <v>38</v>
@@ -905,11 +923,14 @@
       <c r="F4" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>wVq5Sby1x9N</v>
+        <v>cNq8Ywj4v4G</v>
       </c>
       <c r="B5" t="s">
         <v>39</v>
@@ -926,11 +947,14 @@
       <c r="F5" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>xSy5Vcj5x3J</v>
+        <v>iAp3Zxj7r1P</v>
       </c>
       <c r="B6" t="s">
         <v>40</v>
@@ -947,11 +971,14 @@
       <c r="F6" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>wDk2Npl5b6Q</v>
+        <v>sCa9Wqj0s5T</v>
       </c>
       <c r="B7" t="s">
         <v>41</v>
@@ -968,11 +995,14 @@
       <c r="F7" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>hEi1Udl7q5V</v>
+        <v>dTe3Nyc4j5S</v>
       </c>
       <c r="B8" t="s">
         <v>42</v>
@@ -988,6 +1018,9 @@
       </c>
       <c r="F8" t="s">
         <v>72</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -999,8 +1032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
modified erd to include one date per vacancy
</commit_message>
<xml_diff>
--- a/server/db/seeds/Seed_SpreadSheet2.xlsx
+++ b/server/db/seeds/Seed_SpreadSheet2.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="79">
   <si>
     <t>id</t>
   </si>
@@ -635,7 +635,7 @@
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f ca="1">CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>oRv4Fus9w5M</v>
+        <v>aNe4Qiw6l7B</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -671,7 +671,7 @@
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>jQd7Whr5a6H</v>
+        <v>gAa5Jfp1e6R</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
@@ -754,7 +754,7 @@
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f ca="1">CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>lHt9Sci8h2U</v>
+        <v>eIm7Mjy6t6F</v>
       </c>
       <c r="B2" t="s">
         <v>25</v>
@@ -784,7 +784,7 @@
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>nDx7Mgz0h3E</v>
+        <v>hBk7Zos9z6N</v>
       </c>
       <c r="B3" t="s">
         <v>26</v>
@@ -818,10 +818,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="H9" sqref="H9:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -832,7 +832,7 @@
     <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -854,11 +854,17 @@
       <c r="G1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f ca="1">CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>iJi9Mle7a6A</v>
+        <v>kMf7Bxp1b1E</v>
       </c>
       <c r="B2" t="s">
         <v>36</v>
@@ -878,11 +884,17 @@
       <c r="G2" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A8" ca="1" si="0">CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>sDh6Cit5p4O</v>
+        <v>aIi9Tjr6i7V</v>
       </c>
       <c r="B3" t="s">
         <v>37</v>
@@ -902,11 +914,17 @@
       <c r="G3" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>nSm6Icr0i6H</v>
+        <v>tGr0Ilg6c9Q</v>
       </c>
       <c r="B4" t="s">
         <v>38</v>
@@ -926,11 +944,17 @@
       <c r="G4" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>cNq8Ywj4v4G</v>
+        <v>iMl3Qww4s0F</v>
       </c>
       <c r="B5" t="s">
         <v>39</v>
@@ -950,11 +974,17 @@
       <c r="G5" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>iAp3Zxj7r1P</v>
+        <v>fYd7Cpu6e7S</v>
       </c>
       <c r="B6" t="s">
         <v>40</v>
@@ -974,11 +1004,17 @@
       <c r="G6" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>sCa9Wqj0s5T</v>
+        <v>yCw8Sak6z2L</v>
       </c>
       <c r="B7" t="s">
         <v>41</v>
@@ -998,11 +1034,17 @@
       <c r="G7" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>dTe3Nyc4j5S</v>
+        <v>eAj2Mlp0a7T</v>
       </c>
       <c r="B8" t="s">
         <v>42</v>
@@ -1022,6 +1064,16 @@
       <c r="G8" s="2" t="s">
         <v>78</v>
       </c>
+      <c r="H8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1033,7 +1085,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="B9" sqref="B9:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>